<commit_message>
trying local run, but noticed issue with NSNSs
</commit_message>
<xml_diff>
--- a/BHkickReview/BH_kick_reviw.xlsx
+++ b/BHkickReview/BH_kick_reviw.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lvanson/Documents/Projects/Winds2/BHkickReview/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lvanson/Documents/Projects/ZdependentFormEff/BHkickReview/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C123068-78C4-9F46-8F6D-719B622B7052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4D6639C-1EDA-9D45-B84F-5BBE6660CCA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" xr2:uid="{2394415D-BAC6-5B4C-8FC8-E19B3253D939}"/>
   </bookViews>
@@ -128,12 +128,6 @@
     <t>2024MNRAS.527L..82D</t>
   </si>
   <si>
-    <t>https://ui.adsabs.harvard.edu/abs/2021Sci...371.1046M/abstract</t>
-  </si>
-  <si>
-    <t>2021Sci...371.1046M</t>
-  </si>
-  <si>
     <t>﻿IC10 X-1</t>
   </si>
   <si>
@@ -189,6 +183,12 @@
   </si>
   <si>
     <t>2024arXiv240410486G, 2024arXiv240413047E</t>
+  </si>
+  <si>
+    <t>https://ui.adsabs.harvard.edu/abs/2021Sci...371.1046M/abstract, https://arxiv.org/abs/1107.5585</t>
+  </si>
+  <si>
+    <t>2021Sci...371.1046M , 2012ApJ...747..111W</t>
   </si>
 </sst>
 </file>
@@ -611,9 +611,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3330F35D-24B0-1347-B739-3CC9B0CDA4CF}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J13" sqref="J13"/>
+      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -653,7 +653,7 @@
         <v>0</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>5</v>
@@ -724,16 +724,16 @@
         <v>20</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I3" s="2" t="b">
         <v>1</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="2" customFormat="1" ht="22" x14ac:dyDescent="0.3">
@@ -762,7 +762,7 @@
         <v>115</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I4" s="2" t="b">
         <v>0</v>
@@ -798,7 +798,7 @@
         <v>310</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I5" s="2" t="b">
         <v>0</v>
@@ -837,7 +837,7 @@
         <v>114</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I6" s="2" t="b">
         <v>0</v>
@@ -868,14 +868,14 @@
         <v>0</v>
       </c>
       <c r="F7" s="2">
-        <f t="shared" ref="F7:F13" si="1" xml:space="preserve"> MEDIAN(E7,G7)</f>
+        <f t="shared" ref="F7:F12" si="1" xml:space="preserve"> MEDIAN(E7,G7)</f>
         <v>2.5</v>
       </c>
       <c r="G7" s="2">
         <v>5</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I7" s="4" t="b">
         <v>1</v>
@@ -913,7 +913,7 @@
         <v>295</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I8" s="2" t="b">
         <v>0</v>
@@ -927,7 +927,7 @@
     </row>
     <row r="9" spans="1:11" s="2" customFormat="1" ht="22" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B9" s="2">
         <f xml:space="preserve"> MIN(6 - 1, 7.1 -1.3)</f>
@@ -952,21 +952,21 @@
         <v>100</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I9" s="4" t="b">
         <v>1</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:11" s="2" customFormat="1" ht="22" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B10" s="2">
         <v>23</v>
@@ -989,21 +989,21 @@
         <v>130</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I10" s="4" t="b">
         <v>1</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="2" customFormat="1" ht="22" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B11" s="2">
         <f>9.62 - 0.18</f>
@@ -1027,21 +1027,21 @@
         <v>95</v>
       </c>
       <c r="H11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I11" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K11" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="I11" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="2" customFormat="1" ht="22" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B12" s="2">
         <f>8.9 - 0.3</f>
@@ -1065,21 +1065,21 @@
         <v>50</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I12" s="4" t="b">
         <v>0</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="2" customFormat="1" ht="22" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B13" s="2">
         <f xml:space="preserve"> 32.7 - 0.82</f>
@@ -1104,16 +1104,16 @@
         <v>58</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I13" s="4" t="b">
         <v>0</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:11" s="2" customFormat="1" ht="22" x14ac:dyDescent="0.3"/>

</xml_diff>